<commit_message>
check observation values looking at the scale. If multiple values in a cell separated with ; and in a categorical scale, split it in two observations
</commit_message>
<xml_diff>
--- a/vavilov3/tests/data/observations_in_columns.xlsx
+++ b/vavilov3/tests/data/observations_in_columns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t xml:space="preserve">Accession</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">study1</t>
   </si>
   <si>
-    <t xml:space="preserve">red</t>
+    <t xml:space="preserve">1;2</t>
   </si>
   <si>
     <t xml:space="preserve">ESP058:CIAM81001</t>
@@ -122,12 +122,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,7 +159,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -191,10 +195,10 @@
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -205,11 +209,11 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
+      <c r="D3" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,21 +223,21 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>6</v>
+      <c r="C4" s="2" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="2"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="2"/>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="2"/>
+      <c r="J31" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>